<commit_message>
added optimization of energy windows
</commit_message>
<xml_diff>
--- a/efficiency/low_activity/data/backgrounds/HidexAMG-Background Long-016-20230608-122925-AutoExport.xlsx
+++ b/efficiency/low_activity/data/backgrounds/HidexAMG-Background Long-016-20230608-122925-AutoExport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuliy\OneDrive\Documents\Fall 2023\Research\efficiency\low_activity\data\backgrounds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D410A8-D15D-4E87-AC6C-42E20E4CBA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0A4727-D979-4DCF-9EA9-58EFB19B20C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
added new efficiency calculation with optimized energy window
</commit_message>
<xml_diff>
--- a/efficiency/low_activity/data/backgrounds/HidexAMG-Background Long-016-20230608-122925-AutoExport.xlsx
+++ b/efficiency/low_activity/data/backgrounds/HidexAMG-Background Long-016-20230608-122925-AutoExport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuliy\OneDrive\Documents\Fall 2023\Research\efficiency\low_activity\data\backgrounds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0A4727-D979-4DCF-9EA9-58EFB19B20C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01247D7-F6DA-48BE-8648-D6C4E6B62AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>

</xml_diff>